<commit_message>
Updtaing the HSI document after reviewing. Signed-off-by: BasmaAbdelhakim <basmaabdelhakim95@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/HSI_Review.xlsx
+++ b/Input documents/HSI_Review.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>Digital Watch</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>The document already contains block diagram and HW-SW interface is explained in CYRS document.</t>
   </si>
 </sst>
 </file>
@@ -512,12 +518,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -529,36 +565,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -906,200 +912,217 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="8" max="8" width="32.33203125" customWidth="1"/>
+    <col min="8" max="8" width="32.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="24" t="s">
+    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B3" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25" t="s">
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="28"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="26"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="29"/>
-    </row>
-    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="26"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="29"/>
-    </row>
-    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="24" t="s">
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="38"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="39"/>
+    </row>
+    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="36"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="39"/>
+    </row>
+    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="30" t="s">
+      <c r="C6" s="32"/>
+      <c r="D6" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="31"/>
-    </row>
-    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="24" t="s">
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
+    </row>
+    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="30">
+      <c r="C7" s="32"/>
+      <c r="D7" s="24">
         <v>1</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
-    </row>
-    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="24" t="s">
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="25"/>
+    </row>
+    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="30" t="s">
+      <c r="C8" s="32"/>
+      <c r="D8" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="24" t="s">
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="25"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B9" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="30" t="s">
+      <c r="C9" s="32"/>
+      <c r="D9" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="31"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="37"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="39"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="32" t="s">
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="25"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="30"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B11" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="34"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33" t="s">
+      <c r="D12" s="34"/>
+      <c r="E12" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33" t="s">
+      <c r="F12" s="34"/>
+      <c r="G12" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="34"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H12" s="35"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30" t="s">
+      <c r="D13" s="24"/>
+      <c r="E13" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30" t="s">
+      <c r="F13" s="24"/>
+      <c r="G13" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="31"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H13" s="25"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="31"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="25"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="31"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="25"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="31"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="25"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="31"/>
-    </row>
-    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="25"/>
+    </row>
+    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="2"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="36"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -1116,23 +1139,6 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1143,24 +1149,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="100.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="100.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="174.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.26953125" customWidth="1"/>
+    <col min="12" max="12" width="174.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="34.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -1189,7 +1195,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>33</v>
       </c>
@@ -1208,13 +1214,15 @@
       <c r="F2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="10"/>
+      <c r="G2" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="H2" s="10" t="s">
         <v>19</v>
       </c>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>33</v>
       </c>
@@ -1233,16 +1241,20 @@
       <c r="F3" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="H3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="10"/>
+      <c r="I3" s="10" t="s">
+        <v>40</v>
+      </c>
       <c r="K3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>33</v>
       </c>
@@ -1261,13 +1273,18 @@
       <c r="F4" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="10"/>
+      <c r="G4" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="H4" s="10" t="s">
         <v>19</v>
       </c>
       <c r="I4" s="12"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="13"/>
@@ -1281,7 +1298,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="13"/>
@@ -1295,7 +1312,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="13"/>
@@ -1306,7 +1323,7 @@
       <c r="H7" s="10"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="13"/>
@@ -1317,7 +1334,7 @@
       <c r="H8" s="10"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="13"/>
@@ -1334,7 +1351,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="13"/>
@@ -1351,7 +1368,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="13"/>
@@ -1362,7 +1379,7 @@
       <c r="H11" s="10"/>
       <c r="I11" s="12"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="13"/>
@@ -1373,7 +1390,7 @@
       <c r="H12" s="10"/>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="13"/>
@@ -1384,7 +1401,7 @@
       <c r="H13" s="10"/>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="14"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
@@ -1395,7 +1412,7 @@
       <c r="H14" s="10"/>
       <c r="I14" s="19"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -1406,7 +1423,7 @@
       <c r="H15" s="10"/>
       <c r="I15" s="19"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
       <c r="C16" s="16"/>
@@ -1417,7 +1434,7 @@
       <c r="H16" s="10"/>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
       <c r="C17" s="16"/>
@@ -1428,7 +1445,7 @@
       <c r="H17" s="10"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
       <c r="C18" s="16"/>
@@ -1439,7 +1456,7 @@
       <c r="H18" s="10"/>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="14"/>
       <c r="B19" s="15"/>
       <c r="C19" s="16"/>
@@ -1450,7 +1467,7 @@
       <c r="H19" s="10"/>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="14"/>
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
@@ -1461,7 +1478,7 @@
       <c r="H20" s="10"/>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
       <c r="C21" s="16"/>
@@ -1472,7 +1489,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="19"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="14"/>
       <c r="B22" s="15"/>
       <c r="C22" s="16"/>
@@ -1483,7 +1500,7 @@
       <c r="H22" s="10"/>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="14"/>
       <c r="B23" s="15"/>
       <c r="C23" s="16"/>
@@ -1494,7 +1511,7 @@
       <c r="H23" s="10"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="14"/>
       <c r="B24" s="15"/>
       <c r="C24" s="16"/>
@@ -1505,7 +1522,7 @@
       <c r="H24" s="10"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
       <c r="C25" s="16"/>
@@ -1516,7 +1533,7 @@
       <c r="H25" s="10"/>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="16"/>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
@@ -1527,7 +1544,7 @@
       <c r="H26" s="10"/>
       <c r="I26" s="19"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="14"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -1538,7 +1555,7 @@
       <c r="H27" s="10"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="14"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -1549,7 +1566,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="14"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -1560,7 +1577,7 @@
       <c r="H29" s="10"/>
       <c r="I29" s="19"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="16"/>
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
@@ -1571,7 +1588,7 @@
       <c r="H30" s="10"/>
       <c r="I30" s="19"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -1582,7 +1599,7 @@
       <c r="H31" s="10"/>
       <c r="I31" s="19"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="14"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -1593,7 +1610,7 @@
       <c r="H32" s="10"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="16"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
@@ -1604,7 +1621,7 @@
       <c r="H33" s="10"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="16"/>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
@@ -1615,7 +1632,7 @@
       <c r="H34" s="10"/>
       <c r="I34" s="19"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -1626,7 +1643,7 @@
       <c r="H35" s="10"/>
       <c r="I35" s="19"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -1637,7 +1654,7 @@
       <c r="H36" s="10"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
@@ -1648,7 +1665,7 @@
       <c r="H37" s="10"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
@@ -1659,7 +1676,7 @@
       <c r="H38" s="10"/>
       <c r="I38" s="19"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -1670,7 +1687,7 @@
       <c r="H39" s="10"/>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
@@ -1681,7 +1698,7 @@
       <c r="H40" s="10"/>
       <c r="I40" s="19"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="16"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
@@ -1692,7 +1709,7 @@
       <c r="H41" s="10"/>
       <c r="I41" s="19"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="16"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
@@ -1703,7 +1720,7 @@
       <c r="H42" s="10"/>
       <c r="I42" s="19"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="16"/>
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
@@ -1714,7 +1731,7 @@
       <c r="H43" s="10"/>
       <c r="I43" s="19"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="16"/>
       <c r="B44" s="16"/>
       <c r="C44" s="16"/>
@@ -1725,7 +1742,7 @@
       <c r="H44" s="10"/>
       <c r="I44" s="19"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="16"/>
       <c r="B45" s="16"/>
       <c r="C45" s="16"/>
@@ -1756,13 +1773,16 @@
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1 G3:G1048576">
       <formula1>$K$3:$K$3</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
       <formula1>$K$5:$K$6</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+      <formula1>$K$3:$K$4</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating HSI document after reviewing. Signed-off-by: BasmaAbdelhakim <basmaabdelhakim95@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/HSI_Review.xlsx
+++ b/Input documents/HSI_Review.xlsx
@@ -147,7 +147,7 @@
     <t>Accepted</t>
   </si>
   <si>
-    <t>The document already contains block diagram and HW-SW interface is explained in CYRS document.</t>
+    <t>The document  contains block diagram and HW-SW interface is explained in CYRS document.</t>
   </si>
 </sst>
 </file>
@@ -518,12 +518,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -538,33 +565,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -923,206 +923,189 @@
   <sheetData>
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32" t="s">
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="38"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="28"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="39"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="29"/>
     </row>
     <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="39"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="29"/>
     </row>
     <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="24" t="s">
+      <c r="C6" s="25"/>
+      <c r="D6" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31"/>
     </row>
     <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="24">
+      <c r="C7" s="25"/>
+      <c r="D7" s="30">
         <v>1</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="25"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="31"/>
     </row>
     <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="24" t="s">
+      <c r="C8" s="25"/>
+      <c r="D8" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="25"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="24" t="s">
+      <c r="C9" s="25"/>
+      <c r="D9" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="25"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="31"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B10" s="28"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="30"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="39"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="35"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="34"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34" t="s">
+      <c r="D12" s="33"/>
+      <c r="E12" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34" t="s">
+      <c r="F12" s="33"/>
+      <c r="G12" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="35"/>
+      <c r="H12" s="34"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24" t="s">
+      <c r="D13" s="30"/>
+      <c r="E13" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24" t="s">
+      <c r="F13" s="30"/>
+      <c r="G13" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="25"/>
+      <c r="H13" s="31"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="25"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="31"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="25"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="31"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="25"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="25"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="31"/>
     </row>
     <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="2"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="27"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -1139,6 +1122,23 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
Changing the data of V1.4 to be consistent with the history. Signed-off-by: BasmaAbdelhakim <basmaabdelhakim95@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/HSI_Review.xlsx
+++ b/Input documents/HSI_Review.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t xml:space="preserve">Update the status and add one point </t>
+  </si>
+  <si>
+    <t>There was an error in the git tool which lead to the differnce.</t>
   </si>
 </sst>
 </file>
@@ -527,12 +530,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -546,36 +579,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -928,105 +931,105 @@
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="8" max="8" width="32.33203125" customWidth="1"/>
+    <col min="8" max="8" width="32.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="31" t="s">
+    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32" t="s">
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="38"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="39"/>
-    </row>
-    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="39"/>
-    </row>
-    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="31" t="s">
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="28"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="29"/>
+    </row>
+    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="26"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="29"/>
+    </row>
+    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="24" t="s">
+      <c r="C6" s="25"/>
+      <c r="D6" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
-    </row>
-    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="31" t="s">
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31"/>
+    </row>
+    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="24">
+      <c r="C7" s="25"/>
+      <c r="D7" s="30">
         <v>1.4</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="25"/>
-    </row>
-    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="31" t="s">
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="31"/>
+    </row>
+    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="24" t="s">
+      <c r="C8" s="25"/>
+      <c r="D8" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="25"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="31" t="s">
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B9" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="40">
+      <c r="C9" s="25"/>
+      <c r="D9" s="32">
         <v>44076</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="25"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="28"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="30"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="31"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B10" s="38"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="40"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" s="33" t="s">
         <v>4</v>
       </c>
@@ -1037,7 +1040,7 @@
       <c r="G11" s="34"/>
       <c r="H11" s="35"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
@@ -1054,95 +1057,78 @@
       </c>
       <c r="H12" s="35"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24" t="s">
+      <c r="D13" s="30"/>
+      <c r="E13" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24" t="s">
+      <c r="F13" s="30"/>
+      <c r="G13" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="25"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H13" s="31"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B14" s="1">
         <v>0.2</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="40">
+      <c r="D14" s="30"/>
+      <c r="E14" s="32">
         <v>44076</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24" t="s">
+      <c r="F14" s="30"/>
+      <c r="G14" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="25"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H14" s="31"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="25"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="31"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="25"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="25"/>
-    </row>
-    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="31"/>
+    </row>
+    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="2"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="27"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -1159,6 +1145,23 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1169,24 +1172,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="100.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="100.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="34.21875" customWidth="1"/>
-    <col min="12" max="12" width="174.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.1796875" customWidth="1"/>
+    <col min="12" max="12" width="174.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="34.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -1215,7 +1218,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>33</v>
       </c>
@@ -1242,7 +1245,7 @@
       </c>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>33</v>
       </c>
@@ -1274,7 +1277,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>33</v>
       </c>
@@ -1304,7 +1307,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <v>44076</v>
       </c>
@@ -1323,16 +1326,20 @@
       <c r="F5" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="10"/>
+      <c r="G5" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="H5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="12"/>
+      <c r="I5" s="12" t="s">
+        <v>44</v>
+      </c>
       <c r="K5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="13"/>
@@ -1346,7 +1353,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="13"/>
@@ -1357,7 +1364,7 @@
       <c r="H7" s="10"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="13"/>
@@ -1368,7 +1375,7 @@
       <c r="H8" s="10"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="13"/>
@@ -1385,7 +1392,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="13"/>
@@ -1402,7 +1409,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="13"/>
@@ -1413,7 +1420,7 @@
       <c r="H11" s="10"/>
       <c r="I11" s="12"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="13"/>
@@ -1424,7 +1431,7 @@
       <c r="H12" s="10"/>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="13"/>
@@ -1435,7 +1442,7 @@
       <c r="H13" s="10"/>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="14"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
@@ -1446,7 +1453,7 @@
       <c r="H14" s="10"/>
       <c r="I14" s="19"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -1457,7 +1464,7 @@
       <c r="H15" s="10"/>
       <c r="I15" s="19"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
       <c r="C16" s="16"/>
@@ -1468,7 +1475,7 @@
       <c r="H16" s="10"/>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
       <c r="C17" s="16"/>
@@ -1479,7 +1486,7 @@
       <c r="H17" s="10"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
       <c r="C18" s="16"/>
@@ -1490,7 +1497,7 @@
       <c r="H18" s="10"/>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="14"/>
       <c r="B19" s="15"/>
       <c r="C19" s="16"/>
@@ -1501,7 +1508,7 @@
       <c r="H19" s="10"/>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="14"/>
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
@@ -1512,7 +1519,7 @@
       <c r="H20" s="10"/>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
       <c r="C21" s="16"/>
@@ -1523,7 +1530,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="19"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="14"/>
       <c r="B22" s="15"/>
       <c r="C22" s="16"/>
@@ -1534,7 +1541,7 @@
       <c r="H22" s="10"/>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="14"/>
       <c r="B23" s="15"/>
       <c r="C23" s="16"/>
@@ -1545,7 +1552,7 @@
       <c r="H23" s="10"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="14"/>
       <c r="B24" s="15"/>
       <c r="C24" s="16"/>
@@ -1556,7 +1563,7 @@
       <c r="H24" s="10"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
       <c r="C25" s="16"/>
@@ -1567,7 +1574,7 @@
       <c r="H25" s="10"/>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="16"/>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
@@ -1578,7 +1585,7 @@
       <c r="H26" s="10"/>
       <c r="I26" s="19"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="14"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -1589,7 +1596,7 @@
       <c r="H27" s="10"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="14"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -1600,7 +1607,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="14"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -1611,7 +1618,7 @@
       <c r="H29" s="10"/>
       <c r="I29" s="19"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="16"/>
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
@@ -1622,7 +1629,7 @@
       <c r="H30" s="10"/>
       <c r="I30" s="19"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -1633,7 +1640,7 @@
       <c r="H31" s="10"/>
       <c r="I31" s="19"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="14"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -1644,7 +1651,7 @@
       <c r="H32" s="10"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="16"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
@@ -1655,7 +1662,7 @@
       <c r="H33" s="10"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="16"/>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
@@ -1666,7 +1673,7 @@
       <c r="H34" s="10"/>
       <c r="I34" s="19"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -1677,7 +1684,7 @@
       <c r="H35" s="10"/>
       <c r="I35" s="19"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -1688,7 +1695,7 @@
       <c r="H36" s="10"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
@@ -1699,7 +1706,7 @@
       <c r="H37" s="10"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
@@ -1710,7 +1717,7 @@
       <c r="H38" s="10"/>
       <c r="I38" s="19"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -1721,7 +1728,7 @@
       <c r="H39" s="10"/>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
@@ -1732,7 +1739,7 @@
       <c r="H40" s="10"/>
       <c r="I40" s="19"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="16"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
@@ -1743,7 +1750,7 @@
       <c r="H41" s="10"/>
       <c r="I41" s="19"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="16"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
@@ -1754,7 +1761,7 @@
       <c r="H42" s="10"/>
       <c r="I42" s="19"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="16"/>
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
@@ -1765,7 +1772,7 @@
       <c r="H43" s="10"/>
       <c r="I43" s="19"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="16"/>
       <c r="B44" s="16"/>
       <c r="C44" s="16"/>
@@ -1776,7 +1783,7 @@
       <c r="H44" s="10"/>
       <c r="I44" s="19"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="16"/>
       <c r="B45" s="16"/>
       <c r="C45" s="16"/>

</xml_diff>